<commit_message>
Changing to pygame cd4
</commit_message>
<xml_diff>
--- a/QuizGame/src/resources/questionsBase.xlsx
+++ b/QuizGame/src/resources/questionsBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48516\Desktop\QuizGamePythonProject\QuizGame\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A96586-6231-488A-A8CC-30607B3AD3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4DFD23-E07B-4EF6-96A5-AE7510F083F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E6D21BDE-B730-41EF-90B9-093626DC943D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E6D21BDE-B730-41EF-90B9-093626DC943D}"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
   <si>
     <t>PYTANIE</t>
   </si>
@@ -590,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E7B3B8F-AB8D-4B5B-AE63-353814138CE7}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
@@ -709,10 +709,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E327F3B-40D4-4F50-BF3E-6A89688DB474}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,6 +803,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>